<commit_message>
Added picture of SED plot and URL
</commit_message>
<xml_diff>
--- a/data/Sources/MRK1501.xlsx
+++ b/data/Sources/MRK1501.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="MRK1501" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="555">
   <si>
     <t>Results from query to  NASA/IPAC Extragalactic Database (NED),</t>
   </si>
@@ -1676,13 +1676,16 @@
   </si>
   <si>
     <t xml:space="preserve">       151 MHz       </t>
+  </si>
+  <si>
+    <t>http://ned.ipac.caltech.edu/cgi-bin/datasearch?objname=mrk+1501&amp;meas_type=bot&amp;ebars_spec=ebars&amp;label_spec=no&amp;x_spec=freq&amp;y_spec=Fnu_jy&amp;xr=-1&amp;of=table&amp;search_type=Photometry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1817,6 +1820,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2116,7 +2126,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2159,12 +2169,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2198,6 +2213,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2211,6 +2227,55 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>31781</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="http://ned.ipac.caltech.edu/results/photo_7955.png"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5076824" y="28575"/>
+          <a:ext cx="4708557" cy="2847975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2498,53 +2563,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q183"/>
+  <dimension ref="A2:R183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -10873,6 +10943,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>